<commit_message>
Added ERP Module Emp Details pages
</commit_message>
<xml_diff>
--- a/cypress/fixtures/loginData3.xlsx
+++ b/cypress/fixtures/loginData3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\cypress\BankUltimus_Automation\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D48FB17-A5D4-4514-9C5A-DCBCF599375C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC7A904-9558-4C7E-A100-DAD08783F5DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="888" firstSheet="7" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,14 +26,13 @@
     <sheet name="AccountInquary" sheetId="10" r:id="rId11"/>
     <sheet name="AccNominee" sheetId="18" r:id="rId12"/>
     <sheet name="DepoAccBeneficiary" sheetId="21" r:id="rId13"/>
-    <sheet name="EmployeeDetails" sheetId="15" r:id="rId14"/>
+    <sheet name="EmployeeInfo" sheetId="15" r:id="rId14"/>
     <sheet name="DefineCreditLine" sheetId="13" r:id="rId15"/>
     <sheet name="FinProposalRegister" sheetId="14" r:id="rId16"/>
     <sheet name="FinApproval" sheetId="19" r:id="rId17"/>
     <sheet name="FinCommitment" sheetId="20" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -651,7 +650,7 @@
     <t>2005 - Deposit Account Beneficiary</t>
   </si>
   <si>
-    <t>emp-001</t>
+    <t>EMP078</t>
   </si>
 </sst>
 </file>
@@ -1341,7 +1340,7 @@
   <dimension ref="A1:AT2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update demand deposit and inquary page
</commit_message>
<xml_diff>
--- a/cypress/fixtures/loginData3.xlsx
+++ b/cypress/fixtures/loginData3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\cypress\BankUltimus_Automation\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB03FEF-4EFF-404A-9D58-FA2BCFE75BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A3D74D-EFC4-48F5-967B-369AC426EF2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="888" firstSheet="10" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="888" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,6 @@
     <sheet name="FinCommitment" sheetId="20" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -284,9 +283,6 @@
     <t>http://192.168.10.36:4200/sign-in</t>
   </si>
   <si>
-    <t>inzamam</t>
-  </si>
-  <si>
     <t>emp_ID</t>
   </si>
   <si>
@@ -679,6 +675,9 @@
   </si>
   <si>
     <t>605 - PKB_Continuous</t>
+  </si>
+  <si>
+    <t>Anamika</t>
   </si>
 </sst>
 </file>
@@ -1078,8 +1077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1135,10 +1134,10 @@
         <v>75</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>200</v>
       </c>
       <c r="C4">
-        <v>12345</v>
+        <v>123456</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -1146,10 +1145,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B5" t="s">
         <v>190</v>
-      </c>
-      <c r="B5" t="s">
-        <v>191</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1160,10 +1159,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1246,7 +1245,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -1275,84 +1274,84 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" t="s">
         <v>162</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>163</v>
       </c>
-      <c r="C1" t="s">
-        <v>164</v>
-      </c>
       <c r="D1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J1" t="s">
+        <v>100</v>
+      </c>
+      <c r="K1" t="s">
         <v>166</v>
       </c>
-      <c r="G1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H1" t="s">
-        <v>99</v>
-      </c>
-      <c r="I1" t="s">
-        <v>100</v>
-      </c>
-      <c r="J1" t="s">
-        <v>101</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
+        <v>109</v>
+      </c>
+      <c r="M1" t="s">
+        <v>83</v>
+      </c>
+      <c r="N1" t="s">
         <v>167</v>
-      </c>
-      <c r="L1" t="s">
-        <v>110</v>
-      </c>
-      <c r="M1" t="s">
-        <v>84</v>
-      </c>
-      <c r="N1" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>170</v>
-      </c>
-      <c r="B2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C2" t="s">
-        <v>169</v>
-      </c>
-      <c r="D2" t="s">
-        <v>165</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>171</v>
       </c>
       <c r="F2" t="s">
         <v>4</v>
       </c>
       <c r="G2" t="s">
+        <v>171</v>
+      </c>
+      <c r="H2" t="s">
+        <v>176</v>
+      </c>
+      <c r="I2" t="s">
+        <v>177</v>
+      </c>
+      <c r="J2" t="s">
+        <v>177</v>
+      </c>
+      <c r="K2" t="s">
+        <v>171</v>
+      </c>
+      <c r="L2" t="s">
         <v>172</v>
-      </c>
-      <c r="H2" t="s">
-        <v>177</v>
-      </c>
-      <c r="I2" t="s">
-        <v>178</v>
-      </c>
-      <c r="J2" t="s">
-        <v>178</v>
-      </c>
-      <c r="K2" t="s">
-        <v>172</v>
-      </c>
-      <c r="L2" t="s">
-        <v>173</v>
       </c>
       <c r="M2" s="9">
         <v>36841</v>
@@ -1383,27 +1382,27 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B1" t="s">
         <v>184</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>185</v>
       </c>
-      <c r="C1" t="s">
-        <v>186</v>
-      </c>
       <c r="D1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -1447,183 +1446,183 @@
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" t="s">
         <v>77</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>79</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>80</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>81</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>82</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>83</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>84</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>85</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" t="s">
         <v>87</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="P1" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="R1" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="T1" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="V1" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="W1" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="X1" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="Y1" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Z1" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="AA1" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="AA1" s="8" t="s">
+      <c r="AB1" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AC1" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="AC1" s="8" t="s">
+      <c r="AD1" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="AE1" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="AF1" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="AG1" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="AH1" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AI1" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="AD1" s="8" t="s">
+      <c r="AJ1" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK1" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="AL1" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="AM1" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="AN1" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="AO1" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="AP1" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="AE1" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="AF1" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="AG1" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="AH1" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="AI1" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="AJ1" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="AK1" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="AL1" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="AM1" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="AN1" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="AO1" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="AP1" s="8" t="s">
+      <c r="AQ1" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="AQ1" s="8" t="s">
+      <c r="AR1" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="AR1" s="8" t="s">
+      <c r="AS1" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="AS1" s="8" t="s">
+      <c r="AT1" s="8" t="s">
         <v>120</v>
-      </c>
-      <c r="AT1" s="8" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2" t="s">
         <v>122</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>130</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>123</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>131</v>
-      </c>
-      <c r="F2" t="s">
-        <v>124</v>
-      </c>
-      <c r="G2" t="s">
-        <v>132</v>
       </c>
       <c r="H2" s="9">
         <v>33215</v>
       </c>
       <c r="I2" t="s">
+        <v>124</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="K2" t="s">
         <v>125</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="L2" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" t="s">
         <v>127</v>
       </c>
-      <c r="M2" t="s">
-        <v>128</v>
-      </c>
       <c r="N2" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O2">
         <v>5.9</v>
@@ -1632,7 +1631,7 @@
         <v>92</v>
       </c>
       <c r="Q2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="R2" s="9">
         <v>43501</v>
@@ -1770,49 +1769,49 @@
         <v>73</v>
       </c>
       <c r="G1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H1" t="s">
+        <v>135</v>
+      </c>
+      <c r="I1" t="s">
+        <v>138</v>
+      </c>
+      <c r="J1" t="s">
         <v>141</v>
       </c>
-      <c r="H1" t="s">
-        <v>136</v>
-      </c>
-      <c r="I1" t="s">
-        <v>139</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>142</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>143</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>144</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>145</v>
       </c>
-      <c r="N1" t="s">
-        <v>146</v>
-      </c>
       <c r="O1" t="s">
+        <v>147</v>
+      </c>
+      <c r="P1" t="s">
         <v>148</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>149</v>
       </c>
-      <c r="Q1" t="s">
-        <v>150</v>
-      </c>
       <c r="R1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="T1" t="s">
+        <v>151</v>
+      </c>
+      <c r="U1" t="s">
         <v>152</v>
-      </c>
-      <c r="U1" t="s">
-        <v>153</v>
       </c>
       <c r="V1" s="10"/>
     </row>
@@ -1821,7 +1820,7 @@
         <v>1234</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C2">
         <v>876410</v>
@@ -1836,19 +1835,19 @@
         <v>14</v>
       </c>
       <c r="G2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H2" t="s">
+        <v>136</v>
+      </c>
+      <c r="I2" t="s">
+        <v>139</v>
+      </c>
+      <c r="J2" t="s">
         <v>137</v>
       </c>
-      <c r="H2" t="s">
-        <v>137</v>
-      </c>
-      <c r="I2" t="s">
-        <v>140</v>
-      </c>
-      <c r="J2" t="s">
-        <v>138</v>
-      </c>
       <c r="K2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L2" t="s">
         <v>33</v>
@@ -1860,25 +1859,25 @@
         <v>12</v>
       </c>
       <c r="O2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P2">
         <v>12</v>
       </c>
       <c r="Q2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="R2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="S2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="T2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="U2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -1886,7 +1885,7 @@
         <v>1234</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C3">
         <v>93</v>
@@ -1901,19 +1900,19 @@
         <v>19</v>
       </c>
       <c r="G3" t="s">
+        <v>136</v>
+      </c>
+      <c r="H3" t="s">
+        <v>136</v>
+      </c>
+      <c r="I3" t="s">
+        <v>139</v>
+      </c>
+      <c r="J3" t="s">
         <v>137</v>
       </c>
-      <c r="H3" t="s">
-        <v>137</v>
-      </c>
-      <c r="I3" t="s">
-        <v>140</v>
-      </c>
-      <c r="J3" t="s">
-        <v>138</v>
-      </c>
       <c r="K3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L3" t="s">
         <v>33</v>
@@ -1925,38 +1924,38 @@
         <v>12</v>
       </c>
       <c r="O3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P3">
         <v>12</v>
       </c>
       <c r="Q3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="R3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="S3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="T3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="U3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J8" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J11" t="s">
+        <v>197</v>
+      </c>
+      <c r="K11" t="s">
         <v>198</v>
-      </c>
-      <c r="K11" t="s">
-        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -1980,24 +1979,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" t="s">
         <v>179</v>
-      </c>
-      <c r="B1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C1" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -2009,7 +2008,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{553819EE-EFB6-46E5-9349-0EFBBF77EBC3}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
@@ -2023,7 +2022,7 @@
         <v>43</v>
       </c>
       <c r="B1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2036,7 +2035,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2636,7 +2635,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -2652,7 +2651,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -2660,7 +2659,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -2668,7 +2667,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B8">
         <v>6</v>
@@ -2676,7 +2675,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B9">
         <v>7</v>
@@ -2735,7 +2734,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
@@ -2785,7 +2784,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B2">
         <v>100000</v>
@@ -2832,7 +2831,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B2">
         <v>15000</v>

</xml_diff>